<commit_message>
13th - Cleanup and addition of new category
</commit_message>
<xml_diff>
--- a/Reports/MarketBeatRank/2019/T_INV19_BASE/TECHY.xlsx
+++ b/Reports/MarketBeatRank/2019/T_INV19_BASE/TECHY.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="35">
   <si>
     <t>Mar_10</t>
   </si>
@@ -102,6 +102,21 @@
   </si>
   <si>
     <t>Evercore ISI</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mar_13</t>
+  </si>
+  <si>
+    <t>Mar_17</t>
+  </si>
+  <si>
+    <t>Mar_24</t>
+  </si>
+  <si>
+    <t>Mar_27</t>
   </si>
 </sst>
 </file>
@@ -138,8 +153,120 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="113">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -151,9 +278,27 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.0" collapsed="false"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -164,6 +309,18 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -172,6 +329,18 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -180,6 +349,18 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -188,6 +369,18 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -196,6 +389,18 @@
       <c r="B6" t="s">
         <v>2</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -204,6 +409,18 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
+      <c r="C7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -212,6 +429,18 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -220,6 +449,18 @@
       <c r="B9" t="s">
         <v>2</v>
       </c>
+      <c r="C9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -228,6 +469,18 @@
       <c r="B10" t="s">
         <v>2</v>
       </c>
+      <c r="C10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -236,6 +489,18 @@
       <c r="B11" t="s">
         <v>2</v>
       </c>
+      <c r="C11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -244,6 +509,18 @@
       <c r="B12" t="s">
         <v>2</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -252,6 +529,18 @@
       <c r="B13" t="s">
         <v>2</v>
       </c>
+      <c r="C13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -260,6 +549,18 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
+      <c r="C14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -268,6 +569,18 @@
       <c r="B15" t="s">
         <v>2</v>
       </c>
+      <c r="C15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -276,6 +589,18 @@
       <c r="B16" t="s">
         <v>2</v>
       </c>
+      <c r="C16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -284,6 +609,18 @@
       <c r="B17" t="s">
         <v>2</v>
       </c>
+      <c r="C17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -292,6 +629,18 @@
       <c r="B18" t="s">
         <v>2</v>
       </c>
+      <c r="C18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -300,6 +649,18 @@
       <c r="B19" t="s">
         <v>2</v>
       </c>
+      <c r="C19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -308,6 +669,18 @@
       <c r="B20" t="s">
         <v>2</v>
       </c>
+      <c r="C20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -316,6 +689,18 @@
       <c r="B21" t="s">
         <v>2</v>
       </c>
+      <c r="C21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -324,6 +709,18 @@
       <c r="B22" t="s">
         <v>2</v>
       </c>
+      <c r="C22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -332,6 +729,18 @@
       <c r="B23" t="s">
         <v>2</v>
       </c>
+      <c r="C23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -340,6 +749,18 @@
       <c r="B24" t="s">
         <v>2</v>
       </c>
+      <c r="C24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -348,6 +769,18 @@
       <c r="B25" t="s">
         <v>2</v>
       </c>
+      <c r="C25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -356,6 +789,18 @@
       <c r="B26" t="s">
         <v>2</v>
       </c>
+      <c r="C26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -364,6 +809,18 @@
       <c r="B27" t="s">
         <v>2</v>
       </c>
+      <c r="C27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -372,12 +829,36 @@
       <c r="B28" t="s">
         <v>2</v>
       </c>
+      <c r="C28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>